<commit_message>
before running the data
</commit_message>
<xml_diff>
--- a/data/training/Data for summer pictures.xlsx
+++ b/data/training/Data for summer pictures.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>Subjective Color Rating</t>
   </si>
@@ -39,19 +39,184 @@
     <t>Coverage within hue thresholds (30 - 100)</t>
   </si>
   <si>
+    <t>7-4-2014 plot 1.jpg</t>
+  </si>
+  <si>
+    <t>7-4-2014 plot 2.jpg</t>
+  </si>
+  <si>
+    <t>7-4-2014 plot 3.jpg</t>
+  </si>
+  <si>
+    <t>7-4-2014 plot 4.jpg</t>
+  </si>
+  <si>
+    <t>7-4-2014 plot 5.jpg</t>
+  </si>
+  <si>
+    <t>7-4-2014 plot 6.jpg</t>
+  </si>
+  <si>
+    <t>7-4-2014 plot 7.jpg</t>
+  </si>
+  <si>
+    <t>7-4-2014 plot 8.jpg</t>
+  </si>
+  <si>
+    <t>7-4-2014 plot 9.jpg</t>
+  </si>
+  <si>
+    <t>7-4-2014 plot 10.jpg</t>
+  </si>
+  <si>
+    <t>7-4-2014 plot 11.jpg</t>
+  </si>
+  <si>
+    <t>7-4-2014 plot 12.jpg</t>
+  </si>
+  <si>
+    <t>7-17-2014 plot 1.jpg</t>
+  </si>
+  <si>
+    <t>7-17-2014 plot 2.jpg</t>
+  </si>
+  <si>
+    <t>7-17-2014 plot 3.jpg</t>
+  </si>
+  <si>
+    <t>7-17-2014 plot 4.jpg</t>
+  </si>
+  <si>
+    <t>7-17-2014 plot 5.jpg</t>
+  </si>
+  <si>
+    <t>7-17-2014 plot 6.jpg</t>
+  </si>
+  <si>
+    <t>7-17-2014 plot 7.jpg</t>
+  </si>
+  <si>
+    <t>7-17-2014 plot 8.jpg</t>
+  </si>
+  <si>
+    <t>7-17-2014 plot 9.jpg</t>
+  </si>
+  <si>
+    <t>7-17-2014 plot 10.jpg</t>
+  </si>
+  <si>
+    <t>7-17-2014 plot 11.jpg</t>
+  </si>
+  <si>
+    <t>7-17-2014 plot 12.jpg</t>
+  </si>
+  <si>
+    <t>7-31-2014 plot 1.jpg</t>
+  </si>
+  <si>
+    <t>7-31-2014 plot 2.jpg</t>
+  </si>
+  <si>
+    <t>7-31-2014 plot 3.jpg</t>
+  </si>
+  <si>
+    <t>7-31-2014 plot 4.jpg</t>
+  </si>
+  <si>
+    <t>7-31-2014 plot 5.jpg</t>
+  </si>
+  <si>
+    <t>7-31-2014 plot 6.jpg</t>
+  </si>
+  <si>
+    <t>7-31-2014 plot 7.jpg</t>
+  </si>
+  <si>
+    <t>7-31-2014 plot 8.jpg</t>
+  </si>
+  <si>
+    <t>7-31-2014 plot 9.jpg</t>
+  </si>
+  <si>
+    <t>7-31-2014 plot 10.jpg</t>
+  </si>
+  <si>
+    <t>7-31-2014 plot 11.jpg</t>
+  </si>
+  <si>
+    <t>7-31-2014 plot 12.jpg</t>
+  </si>
+  <si>
+    <t>9-25-2014 plot 1.jpg</t>
+  </si>
+  <si>
+    <t>9-25-2014 plot 2.jpg</t>
+  </si>
+  <si>
+    <t>9-25-2014 plot 3.jpg</t>
+  </si>
+  <si>
+    <t>9-25-2014 plot 4.jpg</t>
+  </si>
+  <si>
+    <t>9-25-2014 plot 5.jpg</t>
+  </si>
+  <si>
+    <t>9-25-2014 plot 6.jpg</t>
+  </si>
+  <si>
+    <t>9-25-2014 plot 7.jpg</t>
+  </si>
+  <si>
+    <t>9-25-2014 plot 8.jpg</t>
+  </si>
+  <si>
+    <t>9-25-2014 plot 9.jpg</t>
+  </si>
+  <si>
+    <t>9-25-2014 plot 10.jpg</t>
+  </si>
+  <si>
+    <t>9-25-2014 plot 11.jpg</t>
+  </si>
+  <si>
+    <t>9-25-2014 plot 12.jpg</t>
+  </si>
+  <si>
+    <t>Patch 1-2.jpg</t>
+  </si>
+  <si>
+    <t>Patch 2.jpg</t>
+  </si>
+  <si>
+    <t>Patch 3.jpg</t>
+  </si>
+  <si>
+    <t>Patch 4.jpg</t>
+  </si>
+  <si>
+    <t>Patch 5-2.jpg</t>
+  </si>
+  <si>
+    <t>Patch 6.jpg</t>
+  </si>
+  <si>
+    <t>Patch 7.jpg</t>
+  </si>
+  <si>
+    <t>Patch 8.jpg</t>
+  </si>
+  <si>
+    <t>Patch 9.jpg</t>
+  </si>
+  <si>
+    <t>Patch 10.jpg</t>
+  </si>
+  <si>
+    <t>Patch 11-2.jpg</t>
+  </si>
+  <si>
     <t>File Name</t>
-  </si>
-  <si>
-    <t>7-4-2014 plot 1.jpg</t>
-  </si>
-  <si>
-    <t>9-25-2014 plot 6.jpg</t>
-  </si>
-  <si>
-    <t>Patch 1-2.jpg</t>
-  </si>
-  <si>
-    <t>Patch 6.jpg</t>
   </si>
 </sst>
 </file>
@@ -379,11 +544,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -399,7 +562,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -424,7 +587,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>7.5</v>
@@ -447,75 +610,1339 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>5.25</v>
+        <v>7.25</v>
       </c>
       <c r="C3">
-        <v>5.25</v>
+        <v>7.25</v>
       </c>
       <c r="D3">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="E3">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="F3">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G3" s="2">
-        <v>0.90576699999999999</v>
+        <v>0.95574899999999996</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>7.25</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>7.25</v>
       </c>
       <c r="D4">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="E4">
-        <v>123</v>
+        <v>151</v>
       </c>
       <c r="F4">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="G4" s="2">
-        <v>0.53944700000000001</v>
+        <v>0.94460599999999995</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>7.25</v>
+      </c>
+      <c r="C5">
+        <v>7.25</v>
+      </c>
+      <c r="D5">
+        <v>132</v>
+      </c>
+      <c r="E5">
+        <v>152</v>
+      </c>
+      <c r="F5">
+        <v>96</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.93477500000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B5">
+      <c r="B6">
+        <v>7.25</v>
+      </c>
+      <c r="C6">
+        <v>7.25</v>
+      </c>
+      <c r="D6">
+        <v>134</v>
+      </c>
+      <c r="E6">
+        <v>153</v>
+      </c>
+      <c r="F6">
+        <v>101</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.91248300000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>7.25</v>
+      </c>
+      <c r="C7">
+        <v>7.25</v>
+      </c>
+      <c r="D7">
+        <v>134</v>
+      </c>
+      <c r="E7">
+        <v>151</v>
+      </c>
+      <c r="F7">
+        <v>98</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.91445399999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>7.25</v>
+      </c>
+      <c r="C8">
+        <v>7.25</v>
+      </c>
+      <c r="D8">
+        <v>134</v>
+      </c>
+      <c r="E8">
+        <v>153</v>
+      </c>
+      <c r="F8">
+        <v>99</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.92062999999999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>7.25</v>
+      </c>
+      <c r="C9">
+        <v>7.25</v>
+      </c>
+      <c r="D9">
+        <v>133</v>
+      </c>
+      <c r="E9">
+        <v>152</v>
+      </c>
+      <c r="F9">
+        <v>95</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.91314799999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>7.5</v>
+      </c>
+      <c r="C10">
+        <v>7.5</v>
+      </c>
+      <c r="D10">
+        <v>134</v>
+      </c>
+      <c r="E10">
+        <v>154</v>
+      </c>
+      <c r="F10">
+        <v>97</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.93090399999999995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>7.5</v>
+      </c>
+      <c r="C11">
+        <v>7.5</v>
+      </c>
+      <c r="D11">
+        <v>130</v>
+      </c>
+      <c r="E11">
+        <v>151</v>
+      </c>
+      <c r="F11">
+        <v>93</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.935222</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>7.25</v>
+      </c>
+      <c r="C12">
+        <v>7.25</v>
+      </c>
+      <c r="D12">
+        <v>132</v>
+      </c>
+      <c r="E12">
+        <v>151</v>
+      </c>
+      <c r="F12">
+        <v>96</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0.93310700000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <v>7.25</v>
+      </c>
+      <c r="C13">
+        <v>7.25</v>
+      </c>
+      <c r="D13">
+        <v>130</v>
+      </c>
+      <c r="E13">
+        <v>147</v>
+      </c>
+      <c r="F13">
+        <v>93</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.93562199999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>7.25</v>
+      </c>
+      <c r="D15">
+        <v>131</v>
+      </c>
+      <c r="E15">
+        <v>153</v>
+      </c>
+      <c r="F15">
+        <v>95</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0.92450100000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>6.5</v>
+      </c>
+      <c r="C16">
+        <v>7</v>
+      </c>
+      <c r="D16">
+        <v>135</v>
+      </c>
+      <c r="E16">
+        <v>150</v>
+      </c>
+      <c r="F16">
+        <v>93</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0.92884900000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>7.25</v>
+      </c>
+      <c r="D17">
+        <v>130</v>
+      </c>
+      <c r="E17">
+        <v>145</v>
+      </c>
+      <c r="F17">
+        <v>92</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0.88580400000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>7.25</v>
+      </c>
+      <c r="D18">
+        <v>128</v>
+      </c>
+      <c r="E18">
+        <v>149</v>
+      </c>
+      <c r="F18">
+        <v>89</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0.92216799999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <v>6.75</v>
+      </c>
+      <c r="C19">
+        <v>7</v>
+      </c>
+      <c r="D19">
+        <v>135</v>
+      </c>
+      <c r="E19">
+        <v>149</v>
+      </c>
+      <c r="F19">
+        <v>93</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0.93226799999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20">
+        <v>6.5</v>
+      </c>
+      <c r="C20">
+        <v>7.5</v>
+      </c>
+      <c r="D20">
+        <v>128</v>
+      </c>
+      <c r="E20">
+        <v>144</v>
+      </c>
+      <c r="F20">
+        <v>86</v>
+      </c>
+      <c r="G20" s="2">
+        <v>0.89741000000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21">
+        <v>7.25</v>
+      </c>
+      <c r="C21">
+        <v>7</v>
+      </c>
+      <c r="D21">
+        <v>137</v>
+      </c>
+      <c r="E21">
+        <v>150</v>
+      </c>
+      <c r="F21">
+        <v>98</v>
+      </c>
+      <c r="G21" s="2">
+        <v>0.84725899999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22">
+        <v>6.75</v>
+      </c>
+      <c r="C22">
+        <v>7.25</v>
+      </c>
+      <c r="D22">
+        <v>132</v>
+      </c>
+      <c r="E22">
+        <v>151</v>
+      </c>
+      <c r="F22">
+        <v>94</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0.89936899999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23">
+        <v>6.75</v>
+      </c>
+      <c r="C23">
+        <v>7.25</v>
+      </c>
+      <c r="D23">
+        <v>132</v>
+      </c>
+      <c r="E23">
+        <v>152</v>
+      </c>
+      <c r="F23">
+        <v>93</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0.90869999999999995</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24">
+        <v>7</v>
+      </c>
+      <c r="C24">
+        <v>6.5</v>
+      </c>
+      <c r="D24">
+        <v>128</v>
+      </c>
+      <c r="E24">
+        <v>149</v>
+      </c>
+      <c r="F24">
+        <v>90</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0.922319</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25">
+        <v>6.5</v>
+      </c>
+      <c r="C25">
+        <v>6.75</v>
+      </c>
+      <c r="D25">
+        <v>132</v>
+      </c>
+      <c r="E25">
+        <v>147</v>
+      </c>
+      <c r="F25">
+        <v>90</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0.93319700000000005</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26">
+        <v>6.5</v>
+      </c>
+      <c r="C26">
+        <v>6.75</v>
+      </c>
+      <c r="D26">
+        <v>136</v>
+      </c>
+      <c r="E26">
+        <v>147</v>
+      </c>
+      <c r="F26">
+        <v>94</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0.90555600000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28">
+        <v>7.5</v>
+      </c>
+      <c r="C28">
+        <v>7.5</v>
+      </c>
+      <c r="D28">
+        <v>155</v>
+      </c>
+      <c r="E28">
+        <v>183</v>
+      </c>
+      <c r="F28">
+        <v>137</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0.58464499999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29">
+        <v>6.5</v>
+      </c>
+      <c r="C29">
+        <v>7</v>
+      </c>
+      <c r="D29">
+        <v>149</v>
+      </c>
+      <c r="E29">
+        <v>169</v>
+      </c>
+      <c r="F29">
+        <v>112</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0.99138899999999996</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30">
+        <v>7</v>
+      </c>
+      <c r="C30">
+        <v>7.25</v>
+      </c>
+      <c r="D30">
+        <v>147</v>
+      </c>
+      <c r="E30">
+        <v>170</v>
+      </c>
+      <c r="F30">
+        <v>125</v>
+      </c>
+      <c r="G30" s="2">
+        <v>0.90628399999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31">
+        <v>7</v>
+      </c>
+      <c r="C31">
+        <v>7.25</v>
+      </c>
+      <c r="D31">
+        <v>146</v>
+      </c>
+      <c r="E31">
+        <v>172</v>
+      </c>
+      <c r="F31">
+        <v>124</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0.83382000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32">
+        <v>6.75</v>
+      </c>
+      <c r="C32">
+        <v>7</v>
+      </c>
+      <c r="D32">
+        <v>145</v>
+      </c>
+      <c r="E32">
+        <v>166</v>
+      </c>
+      <c r="F32">
+        <v>116</v>
+      </c>
+      <c r="G32" s="2">
+        <v>0.95447800000000005</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33">
+        <v>6.5</v>
+      </c>
+      <c r="C33">
+        <v>7</v>
+      </c>
+      <c r="D33">
+        <v>144</v>
+      </c>
+      <c r="E33">
+        <v>162</v>
+      </c>
+      <c r="F33">
+        <v>104</v>
+      </c>
+      <c r="G33" s="2">
+        <v>0.99576299999999995</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34">
+        <v>7.25</v>
+      </c>
+      <c r="C34">
+        <v>7.5</v>
+      </c>
+      <c r="D34">
+        <v>156</v>
+      </c>
+      <c r="E34">
+        <v>177</v>
+      </c>
+      <c r="F34">
+        <v>125</v>
+      </c>
+      <c r="G34" s="2">
+        <v>0.98739699999999997</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35">
+        <v>6.75</v>
+      </c>
+      <c r="C35">
+        <v>7</v>
+      </c>
+      <c r="D35">
+        <v>171</v>
+      </c>
+      <c r="E35">
+        <v>190</v>
+      </c>
+      <c r="F35">
+        <v>134</v>
+      </c>
+      <c r="G35" s="2">
+        <v>0.99685400000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36">
+        <v>6.75</v>
+      </c>
+      <c r="C36">
+        <v>7.25</v>
+      </c>
+      <c r="D36">
+        <v>162</v>
+      </c>
+      <c r="E36">
+        <v>186</v>
+      </c>
+      <c r="F36">
+        <v>125</v>
+      </c>
+      <c r="G36" s="2">
+        <v>0.99195299999999997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37">
+        <v>7</v>
+      </c>
+      <c r="C37">
+        <v>7.25</v>
+      </c>
+      <c r="D37">
+        <v>171</v>
+      </c>
+      <c r="E37">
+        <v>191</v>
+      </c>
+      <c r="F37">
+        <v>134</v>
+      </c>
+      <c r="G37" s="2">
+        <v>0.99478500000000003</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38">
+        <v>6.5</v>
+      </c>
+      <c r="C38">
+        <v>6.5</v>
+      </c>
+      <c r="D38">
+        <v>143</v>
+      </c>
+      <c r="E38">
+        <v>163</v>
+      </c>
+      <c r="F38">
+        <v>103</v>
+      </c>
+      <c r="G38" s="2">
+        <v>0.997529</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39">
+        <v>6.5</v>
+      </c>
+      <c r="C39">
+        <v>6.75</v>
+      </c>
+      <c r="D39">
+        <v>151</v>
+      </c>
+      <c r="E39">
+        <v>167</v>
+      </c>
+      <c r="F39">
+        <v>110</v>
+      </c>
+      <c r="G39" s="2">
+        <v>0.99682099999999996</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41">
+        <v>7.5</v>
+      </c>
+      <c r="C41">
+        <v>7.5</v>
+      </c>
+      <c r="D41">
+        <v>130</v>
+      </c>
+      <c r="E41">
+        <v>153</v>
+      </c>
+      <c r="F41">
+        <v>94</v>
+      </c>
+      <c r="G41" s="2">
+        <v>0.869309</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42">
+        <v>6.5</v>
+      </c>
+      <c r="C42">
+        <v>6.5</v>
+      </c>
+      <c r="D42">
+        <v>135</v>
+      </c>
+      <c r="E42">
+        <v>146</v>
+      </c>
+      <c r="F42">
+        <v>94</v>
+      </c>
+      <c r="G42" s="2">
+        <v>0.89442500000000003</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43">
+        <v>5.25</v>
+      </c>
+      <c r="C43">
+        <v>5.25</v>
+      </c>
+      <c r="D43">
+        <v>138</v>
+      </c>
+      <c r="E43">
+        <v>146</v>
+      </c>
+      <c r="F43">
+        <v>92</v>
+      </c>
+      <c r="G43" s="2">
+        <v>0.91149500000000006</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44">
+        <v>6.75</v>
+      </c>
+      <c r="C44">
+        <v>6.75</v>
+      </c>
+      <c r="D44">
+        <v>132</v>
+      </c>
+      <c r="E44">
+        <v>152</v>
+      </c>
+      <c r="F44">
+        <v>94</v>
+      </c>
+      <c r="G44" s="2">
+        <v>0.91011600000000004</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45">
+        <v>5.75</v>
+      </c>
+      <c r="C45">
+        <v>5.75</v>
+      </c>
+      <c r="D45">
+        <v>137</v>
+      </c>
+      <c r="E45">
+        <v>149</v>
+      </c>
+      <c r="F45">
+        <v>90</v>
+      </c>
+      <c r="G45" s="2">
+        <v>0.93595200000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46">
+        <v>5.25</v>
+      </c>
+      <c r="C46">
+        <v>5.25</v>
+      </c>
+      <c r="D46">
+        <v>142</v>
+      </c>
+      <c r="E46">
+        <v>147</v>
+      </c>
+      <c r="F46">
+        <v>96</v>
+      </c>
+      <c r="G46" s="2">
+        <v>0.90576699999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47">
+        <v>6</v>
+      </c>
+      <c r="C47">
+        <v>6</v>
+      </c>
+      <c r="D47">
+        <v>134</v>
+      </c>
+      <c r="E47">
+        <v>148</v>
+      </c>
+      <c r="F47">
+        <v>92</v>
+      </c>
+      <c r="G47" s="2">
+        <v>0.90309899999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48">
+        <v>6.25</v>
+      </c>
+      <c r="C48">
+        <v>6.25</v>
+      </c>
+      <c r="D48">
+        <v>136</v>
+      </c>
+      <c r="E48">
+        <v>149</v>
+      </c>
+      <c r="F48">
+        <v>94</v>
+      </c>
+      <c r="G48" s="2">
+        <v>0.88598500000000002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49">
+        <v>7</v>
+      </c>
+      <c r="C49">
+        <v>7</v>
+      </c>
+      <c r="D49">
+        <v>132</v>
+      </c>
+      <c r="E49">
+        <v>154</v>
+      </c>
+      <c r="F49">
+        <v>92</v>
+      </c>
+      <c r="G49" s="2">
+        <v>0.90813200000000005</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50">
+        <v>7</v>
+      </c>
+      <c r="C50">
+        <v>7</v>
+      </c>
+      <c r="D50">
+        <v>130</v>
+      </c>
+      <c r="E50">
+        <v>152</v>
+      </c>
+      <c r="F50">
+        <v>91</v>
+      </c>
+      <c r="G50" s="2">
+        <v>0.89838799999999996</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51">
+        <v>5.5</v>
+      </c>
+      <c r="C51">
+        <v>5.5</v>
+      </c>
+      <c r="D51">
+        <v>139</v>
+      </c>
+      <c r="E51">
+        <v>148</v>
+      </c>
+      <c r="F51">
+        <v>93</v>
+      </c>
+      <c r="G51" s="2">
+        <v>0.93591999999999997</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
+        <v>53</v>
+      </c>
+      <c r="B52">
         <v>4</v>
       </c>
-      <c r="C5">
+      <c r="C52">
         <v>4</v>
       </c>
-      <c r="D5">
+      <c r="D52">
+        <v>142</v>
+      </c>
+      <c r="E52">
+        <v>145</v>
+      </c>
+      <c r="F52">
+        <v>92</v>
+      </c>
+      <c r="G52" s="2">
+        <v>0.93331299999999995</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>2</v>
+      </c>
+      <c r="C55">
+        <v>2</v>
+      </c>
+      <c r="D55">
+        <v>138</v>
+      </c>
+      <c r="E55">
+        <v>123</v>
+      </c>
+      <c r="F55">
+        <v>106</v>
+      </c>
+      <c r="G55" s="2">
+        <v>0.53944700000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>3</v>
+      </c>
+      <c r="C56">
+        <v>3</v>
+      </c>
+      <c r="D56">
+        <v>139</v>
+      </c>
+      <c r="E56">
+        <v>129</v>
+      </c>
+      <c r="F56">
+        <v>106</v>
+      </c>
+      <c r="G56" s="2">
+        <v>0.72775000000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>135</v>
+      </c>
+      <c r="E57">
+        <v>122</v>
+      </c>
+      <c r="F57">
+        <v>105</v>
+      </c>
+      <c r="G57" s="2">
+        <v>0.59547000000000005</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>4</v>
+      </c>
+      <c r="C58">
+        <v>3</v>
+      </c>
+      <c r="D58">
         <v>136</v>
       </c>
-      <c r="E5">
+      <c r="E58">
+        <v>127</v>
+      </c>
+      <c r="F58">
+        <v>103</v>
+      </c>
+      <c r="G58" s="2">
+        <v>0.71528899999999995</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>3</v>
+      </c>
+      <c r="C59">
+        <v>2.5</v>
+      </c>
+      <c r="D59">
+        <v>128</v>
+      </c>
+      <c r="E59">
+        <v>122</v>
+      </c>
+      <c r="F59">
+        <v>91</v>
+      </c>
+      <c r="G59" s="2">
+        <v>0.84254099999999998</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>4</v>
+      </c>
+      <c r="C60">
+        <v>4</v>
+      </c>
+      <c r="D60">
+        <v>136</v>
+      </c>
+      <c r="E60">
         <v>131</v>
       </c>
-      <c r="F5">
+      <c r="F60">
         <v>102</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G60" s="2">
         <v>0.79179999999999995</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <v>7.5</v>
+      </c>
+      <c r="C61">
+        <v>8</v>
+      </c>
+      <c r="D61">
+        <v>118</v>
+      </c>
+      <c r="E61">
+        <v>135</v>
+      </c>
+      <c r="F61">
+        <v>77</v>
+      </c>
+      <c r="G61" s="2">
+        <v>0.88771699999999998</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A62" t="s">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <v>7.5</v>
+      </c>
+      <c r="C62">
+        <v>8</v>
+      </c>
+      <c r="D62">
+        <v>118</v>
+      </c>
+      <c r="E62">
+        <v>136</v>
+      </c>
+      <c r="F62">
+        <v>89</v>
+      </c>
+      <c r="G62" s="2">
+        <v>0.77693599999999996</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A63" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63">
+        <v>5.5</v>
+      </c>
+      <c r="C63">
+        <v>3.5</v>
+      </c>
+      <c r="D63">
+        <v>120</v>
+      </c>
+      <c r="E63">
+        <v>137</v>
+      </c>
+      <c r="F63">
+        <v>84</v>
+      </c>
+      <c r="G63" s="2">
+        <v>0.84872300000000001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A64" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64">
+        <v>3.5</v>
+      </c>
+      <c r="C64">
+        <v>3.5</v>
+      </c>
+      <c r="D64">
+        <v>126</v>
+      </c>
+      <c r="E64">
+        <v>130</v>
+      </c>
+      <c r="F64">
+        <v>93</v>
+      </c>
+      <c r="G64" s="2">
+        <v>0.90892300000000004</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A65" t="s">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <v>6.25</v>
+      </c>
+      <c r="C65">
+        <v>4</v>
+      </c>
+      <c r="D65">
+        <v>123</v>
+      </c>
+      <c r="E65">
+        <v>131</v>
+      </c>
+      <c r="F65">
+        <v>110</v>
+      </c>
+      <c r="G65" s="2">
+        <v>0.50801499999999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>